<commit_message>
visit_source_key 항목 구분되도록 변경, visit_source_key를 최대한 PID + INDD(ORDDD) + CRETNO + INSTCD로 구성 안될경우 컬럼 하나씩 빼는 방법적용
</commit_message>
<xml_diff>
--- a/KNUH/감염병 CDM ETL정의서_경북대.xlsx
+++ b/KNUH/감염병 CDM ETL정의서_경북대.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\jbcd\Infectious_CDM\KNUH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B87B7A-90BB-42C1-A7E4-8D04CE151A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E77EF-C6BC-4F3B-9FE5-573B0181DFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="855" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATION" sheetId="2" r:id="rId1"/>
@@ -3437,11 +3437,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3449,29 +3449,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3482,22 +3482,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -3994,7 +3994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
@@ -4052,19 +4052,19 @@
       <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="68" t="s">
         <v>304</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -4075,11 +4075,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="79"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="49" t="s">
         <v>471</v>
       </c>
@@ -4088,11 +4088,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="79"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="49" t="s">
         <v>478</v>
       </c>
@@ -4101,11 +4101,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="71"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="80"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="49" t="s">
         <v>613</v>
       </c>
@@ -4135,16 +4135,16 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="14" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="71" t="s">
         <v>245</v>
       </c>
       <c r="E8" s="74" t="s">
@@ -4158,10 +4158,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="14" customFormat="1" ht="134.4" x14ac:dyDescent="0.4">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="75"/>
       <c r="F9" s="49" t="s">
         <v>471</v>
@@ -4171,10 +4171,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A10" s="77"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="75"/>
       <c r="F10" s="49" t="s">
         <v>479</v>
@@ -4184,10 +4184,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="76"/>
       <c r="F11" s="49" t="s">
         <v>613</v>
@@ -4197,14 +4197,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="14" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70" t="s">
+      <c r="C12" s="71"/>
+      <c r="D12" s="71" t="s">
         <v>246</v>
       </c>
       <c r="E12" s="74" t="s">
@@ -4218,10 +4218,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="75"/>
       <c r="F13" s="49" t="s">
         <v>471</v>
@@ -4231,10 +4231,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="75"/>
       <c r="F14" s="49" t="s">
         <v>478</v>
@@ -4244,10 +4244,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="77"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="76"/>
       <c r="F15" s="49" t="s">
         <v>613</v>
@@ -4257,14 +4257,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="14" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70" t="s">
+      <c r="C16" s="71"/>
+      <c r="D16" s="71" t="s">
         <v>247</v>
       </c>
       <c r="E16" s="74" t="s">
@@ -4278,10 +4278,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="75"/>
       <c r="F17" s="49" t="s">
         <v>471</v>
@@ -4291,10 +4291,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="75"/>
       <c r="F18" s="49" t="s">
         <v>478</v>
@@ -4304,10 +4304,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="76"/>
       <c r="F19" s="49" t="s">
         <v>613</v>
@@ -4317,14 +4317,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="14" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="71" t="s">
         <v>242</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70" t="s">
+      <c r="C20" s="71"/>
+      <c r="D20" s="71" t="s">
         <v>248</v>
       </c>
       <c r="E20" s="74" t="s">
@@ -4338,10 +4338,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="14" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="75"/>
       <c r="F21" s="49" t="s">
         <v>478</v>
@@ -4351,10 +4351,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" s="14" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="71"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="76"/>
       <c r="F22" s="49" t="s">
         <v>613</v>
@@ -4448,17 +4448,17 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="14" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="70" t="s">
+      <c r="C27" s="80"/>
+      <c r="D27" s="71" t="s">
         <v>250</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="77" t="s">
         <v>367</v>
       </c>
       <c r="F27" s="53" t="s">
@@ -4469,11 +4469,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" s="14" customFormat="1" ht="134.4" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="69"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="79"/>
       <c r="F28" s="49" t="s">
         <v>471</v>
       </c>
@@ -4604,19 +4604,19 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="14" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A35" s="72" t="s">
+      <c r="A35" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="72" t="s">
+      <c r="C35" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="70" t="s">
+      <c r="D35" s="71" t="s">
         <v>255</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="77" t="s">
         <v>360</v>
       </c>
       <c r="F35" s="53" t="s">
@@ -4627,11 +4627,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="14" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A36" s="82"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="81"/>
+      <c r="A36" s="81"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="49" t="s">
         <v>471</v>
       </c>
@@ -4640,11 +4640,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="14" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="69"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="79"/>
       <c r="F37" s="53" t="s">
         <v>432</v>
       </c>
@@ -4714,17 +4714,17 @@
       <c r="G40" s="48"/>
     </row>
     <row r="41" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70" t="s">
+      <c r="C41" s="71"/>
+      <c r="D41" s="71" t="s">
         <v>257</v>
       </c>
-      <c r="E41" s="78" t="s">
+      <c r="E41" s="68" t="s">
         <v>371</v>
       </c>
       <c r="F41" s="49" t="s">
@@ -4735,11 +4735,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" s="14" customFormat="1" ht="134.4" x14ac:dyDescent="0.4">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="79"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="49" t="s">
         <v>471</v>
       </c>
@@ -4748,11 +4748,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="79"/>
+      <c r="A43" s="72"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="49" t="s">
         <v>479</v>
       </c>
@@ -4761,11 +4761,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A44" s="71"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="80"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="70"/>
       <c r="F44" s="49" t="s">
         <v>613</v>
       </c>
@@ -5217,46 +5217,46 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
     <mergeCell ref="E41:E44"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="C41:C44"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5268,7 +5268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -6393,8 +6393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="A14:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7481,7 +7481,7 @@
       <c r="D3" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="66" t="s">
         <v>304</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -7496,7 +7496,7 @@
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
-      <c r="E4" s="63"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="1" t="s">
         <v>482</v>
       </c>
@@ -7572,7 +7572,7 @@
       <c r="D8" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="62" t="s">
         <v>327</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -7587,7 +7587,7 @@
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
       <c r="D9" s="59"/>
-      <c r="E9" s="67"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="1" t="s">
         <v>482</v>
       </c>
@@ -7792,7 +7792,7 @@
       <c r="F20" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="62" t="s">
         <v>466</v>
       </c>
     </row>
@@ -7805,7 +7805,7 @@
       <c r="F21" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G21" s="67"/>
+      <c r="G21" s="63"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="58" t="s">
@@ -7824,7 +7824,7 @@
       <c r="F22" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="62" t="s">
         <v>468</v>
       </c>
     </row>
@@ -7837,7 +7837,7 @@
       <c r="F23" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G23" s="67"/>
+      <c r="G23" s="63"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="58" t="s">
@@ -7858,7 +7858,7 @@
       <c r="F24" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="62" t="s">
         <v>468</v>
       </c>
     </row>
@@ -7871,7 +7871,7 @@
       <c r="F25" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G25" s="67"/>
+      <c r="G25" s="63"/>
     </row>
     <row r="26" spans="1:7" ht="78" x14ac:dyDescent="0.4">
       <c r="A26" s="29" t="s">
@@ -8041,6 +8041,43 @@
     <row r="35" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="G24:G25"/>
@@ -8057,43 +8094,6 @@
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8649,8 +8649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="E9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9211,7 +9211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>